<commit_message>
added nursing demand full functionality
</commit_message>
<xml_diff>
--- a/data/MoH_Model_Input.xlsx
+++ b/data/MoH_Model_Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharifKanaan\Documents\MSE Documents\Projects\MoH WFP Nurses\moh-nurses-wfp-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC1F5A9-0AD1-41B5-AAB6-00B58031DC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41F2387-F512-4D00-B2F6-10BAC1074337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="897" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="897" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nursing Services" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Scenarios" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Demand Data by Speciality'!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Demand Data by Speciality'!$A$1:$W$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="137">
   <si>
     <t>Outpatient Services</t>
   </si>
@@ -442,6 +442,18 @@
   </si>
   <si>
     <t>High Scenario</t>
+  </si>
+  <si>
+    <t>Selected Driver</t>
+  </si>
+  <si>
+    <t>Technician %</t>
+  </si>
+  <si>
+    <t>Registered Nurse %</t>
+  </si>
+  <si>
+    <t>APRN %</t>
   </si>
 </sst>
 </file>
@@ -485,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -498,6 +510,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -780,358 +795,880 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.21875" customWidth="1"/>
     <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F35" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>45</v>
       </c>
       <c r="B40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F41" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43" t="s">
         <v>49</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E43" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="6">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -1143,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED3763B-DC16-43D2-BDDF-ACB9BFDBD5FA}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,7 +1868,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B23"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1883,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8260C5-3A41-46D3-8671-E5809231BD4F}">
   <dimension ref="A1:W127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1922,7 +2459,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>93</v>
@@ -10932,6 +11469,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W127" xr:uid="{AF8260C5-3A41-46D3-8671-E5809231BD4F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10941,7 +11479,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10992,7 +11530,7 @@
         <v>132</v>
       </c>
       <c r="C4" s="3">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>